<commit_message>
fixed bug in ExcelDoc.Proces(DocState, DirectoryInfo) where the original file instead of the target file was processed.
</commit_message>
<xml_diff>
--- a/QmsHero/QmsDoc.Test/Fixtures/Active QMS Documents/SOP-001 Quality Manual Documents/F-001B Document Control Index Rev2.xlsx
+++ b/QmsHero/QmsDoc.Test/Fixtures/Active QMS Documents/SOP-001 Quality Manual Documents/F-001B Document Control Index Rev2.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <fileSharing readOnlyRecommended="1" userName="Lean RAQA Systems" algorithmName="SHA-512" hashValue="bzDIcT67keNthI6RyMCjJIZ7DRgmCt95B3WvZETTe7ButBYjUWkD/jtcCzlxwVYsJkpX3kvGXMDsU4/EIfj3UQ==" saltValue="++8SSdgLcx56wxolwAEJsg==" spinCount="100000"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Box Sync\CF - GT Medical\Draft Documents (Review)\DCN-010\SOP-001 Quality Manual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raine\Documents\Dev\qmsHero\QmsHero\QmsDoc.Test\Fixtures\Active QMS Documents\SOP-001 Quality Manual Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7961A601-62F1-457D-A676-A24B21F72780}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{AC4CAC1B-34B1-4E86-8EFB-A36BF99A6D4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11565" windowHeight="6315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4308" yWindow="2724" windowWidth="30960" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Control Index (F-001B)" sheetId="1" r:id="rId1"/>
@@ -611,22 +611,22 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="59.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="13" style="7" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.85546875" style="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
@@ -641,77 +641,77 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>

</xml_diff>

<commit_message>
Word and ExcelDoc now return new Doc when targetDir overload is used, preventing confusing with doc.FileInfo state changes, and removing need to maintain inner targetFile and targetDir fields on the docs.
</commit_message>
<xml_diff>
--- a/QmsHero/QmsDoc.Test/Fixtures/Active QMS Documents/SOP-001 Quality Manual Documents/F-001B Document Control Index Rev2.xlsx
+++ b/QmsHero/QmsDoc.Test/Fixtures/Active QMS Documents/SOP-001 Quality Manual Documents/F-001B Document Control Index Rev2.xlsx
@@ -604,133 +604,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:E12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13" style="7" customWidth="1"/>
-    <col min="6" max="6" width="14" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="97" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader xml:space="preserve">&amp;L&amp;G&amp;C&amp;"Arial,Regular"&amp;10DOCUMENT NAME: &amp;"Arial,Bold"Document Control Index (F-001B)&amp;R&amp;"Arial,Regular"&amp;10&amp;K000000Effective Date: 2018-11-26 
-Revision: 2 </oddHeader>
-    <oddFooter>&amp;R&amp;"Arial,Normal"&amp;10Page &amp;P of &amp;N</oddFooter>
-  </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:pageSetUpPr fitToPage="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:E12"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <x:selection activeCell="C5" sqref="C5"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="2.6640625" style="6" customWidth="1"/>
+    <x:col min="2" max="2" width="7.44140625" style="1" customWidth="1"/>
+    <x:col min="3" max="3" width="59.88671875" style="1" customWidth="1"/>
+    <x:col min="4" max="4" width="9.33203125" style="2" customWidth="1"/>
+    <x:col min="5" max="5" width="13" style="7" customWidth="1"/>
+    <x:col min="6" max="6" width="14" style="1" customWidth="1"/>
+    <x:col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
+    <x:col min="8" max="16384" width="10.88671875" style="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="12" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B1" s="13"/>
+      <x:c r="C1" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D1" s="4" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E1" s="5" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="10"/>
+      <x:c r="B2" s="10"/>
+      <x:c r="C2" s="10"/>
+      <x:c r="D2" s="11"/>
+      <x:c r="E2" s="11"/>
+    </x:row>
+    <x:row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="10"/>
+      <x:c r="B3" s="10"/>
+      <x:c r="C3" s="10"/>
+      <x:c r="D3" s="11"/>
+      <x:c r="E3" s="11"/>
+    </x:row>
+    <x:row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="10"/>
+      <x:c r="B4" s="10"/>
+      <x:c r="C4" s="10"/>
+      <x:c r="D4" s="11"/>
+      <x:c r="E4" s="11"/>
+    </x:row>
+    <x:row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="10"/>
+      <x:c r="B5" s="10"/>
+      <x:c r="C5" s="10"/>
+      <x:c r="D5" s="11"/>
+      <x:c r="E5" s="11"/>
+    </x:row>
+    <x:row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="10"/>
+      <x:c r="B6" s="10"/>
+      <x:c r="C6" s="10"/>
+      <x:c r="D6" s="11"/>
+      <x:c r="E6" s="11"/>
+    </x:row>
+    <x:row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="10"/>
+      <x:c r="B7" s="10"/>
+      <x:c r="C7" s="10"/>
+      <x:c r="D7" s="11"/>
+      <x:c r="E7" s="11"/>
+    </x:row>
+    <x:row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="10"/>
+      <x:c r="B8" s="10"/>
+      <x:c r="C8" s="10"/>
+      <x:c r="D8" s="11"/>
+      <x:c r="E8" s="11"/>
+    </x:row>
+    <x:row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="10"/>
+      <x:c r="B9" s="10"/>
+      <x:c r="C9" s="10"/>
+      <x:c r="D9" s="11"/>
+      <x:c r="E9" s="11"/>
+    </x:row>
+    <x:row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="10"/>
+      <x:c r="B10" s="10"/>
+      <x:c r="C10" s="10"/>
+      <x:c r="D10" s="11"/>
+      <x:c r="E10" s="11"/>
+    </x:row>
+    <x:row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="10"/>
+      <x:c r="B11" s="10"/>
+      <x:c r="C11" s="10"/>
+      <x:c r="D11" s="11"/>
+      <x:c r="E11" s="11"/>
+    </x:row>
+    <x:row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <x:c r="A12" s="10"/>
+      <x:c r="B12" s="10"/>
+      <x:c r="C12" s="10"/>
+      <x:c r="D12" s="11"/>
+      <x:c r="E12" s="11"/>
+    </x:row>
+  </x:sheetData>
+  <x:mergeCells count="1">
+    <x:mergeCell ref="A1:B1"/>
+  </x:mergeCells>
+  <x:phoneticPr fontId="4" type="noConversion"/>
+  <x:printOptions horizontalCentered="1"/>
+  <x:pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <x:pageSetup scale="97" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <x:headerFooter alignWithMargins="0">
+    <x:oddHeader xml:space="preserve">&amp;L&amp;G&amp;C&amp;"Arial,Regular"&amp;10DOCUMENT NAME: &amp;"Arial,Bold"Document Control Index (F-001B)&amp;R&amp;"Arial,Regular"&amp;10&amp;K000000Effective Date: 2018-11-26 
+Revision: 2 </x:oddHeader>
+    <x:oddFooter>&amp;R&amp;"Arial,Normal"&amp;10Page &amp;P of &amp;N</x:oddFooter>
+  </x:headerFooter>
+  <x:legacyDrawingHF r:id="rId2"/>
+</x:worksheet>
 </file>
</xml_diff>